<commit_message>
commit just before python application webinar on 2024-0527
</commit_message>
<xml_diff>
--- a/c3_data/data/df.xlsx
+++ b/c3_data/data/df.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27716"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\python3\kosmes\3.data\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\python3\repos\pykosmes\c3_data\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC3CF2FF-55FA-4E61-9180-C7A07DFABA43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCFBF2B-905C-42EE-9C44-26E515E8F289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>c0</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>r2</t>
+  </si>
+  <si>
+    <t>df.xlsx</t>
   </si>
 </sst>
 </file>
@@ -54,6 +57,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -98,7 +102,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -400,11 +404,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="340" zoomScaleNormal="340" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="340" zoomScaleNormal="340" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>